<commit_message>
Don't save new Row elements in SheetData when they are 'empty' (no child cells or no styles)
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Comments/AddingComments.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Comments/AddingComments.xlsx
@@ -1201,21 +1201,15 @@
         <x:v>3</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:11"/>
-    <x:row r="6" spans="1:11"/>
     <x:row r="7" spans="1:11">
       <x:c r="E7" s="0" t="s"/>
     </x:row>
-    <x:row r="8" spans="1:11"/>
     <x:row r="9" spans="1:11">
       <x:c r="A9" s="0" t="s"/>
       <x:c r="D9" s="0" t="s"/>
       <x:c r="E9" s="0" t="s"/>
       <x:c r="F9" s="0" t="s"/>
     </x:row>
-    <x:row r="10" spans="1:11"/>
-    <x:row r="11" spans="1:11"/>
-    <x:row r="12" spans="1:11"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
@@ -1240,15 +1234,12 @@
     <x:col min="1" max="5" width="9.140625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:5"/>
     <x:row r="2" spans="1:5">
       <x:c r="A2" s="0" t="s"/>
     </x:row>
-    <x:row r="3" spans="1:5"/>
     <x:row r="4" spans="1:5">
       <x:c r="A4" s="0" t="s"/>
     </x:row>
-    <x:row r="5" spans="1:5"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
@@ -1276,9 +1267,6 @@
     <x:row r="1" spans="1:4">
       <x:c r="A1" s="0" t="s"/>
     </x:row>
-    <x:row r="2" spans="1:4"/>
-    <x:row r="3" spans="1:4"/>
-    <x:row r="4" spans="1:4"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
@@ -1318,9 +1306,6 @@
     <x:row r="4" spans="1:4">
       <x:c r="A4" s="0" t="s"/>
     </x:row>
-    <x:row r="5" spans="1:4"/>
-    <x:row r="6" spans="1:4"/>
-    <x:row r="7" spans="1:4"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
@@ -1348,11 +1333,6 @@
     <x:row r="1" spans="1:5">
       <x:c r="A1" s="0" t="s"/>
     </x:row>
-    <x:row r="5" spans="1:5"/>
-    <x:row r="6" spans="1:5"/>
-    <x:row r="7" spans="1:5"/>
-    <x:row r="8" spans="1:5"/>
-    <x:row r="9" spans="1:5"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
@@ -1377,13 +1357,9 @@
     <x:col min="1" max="4" width="9.140625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:4"/>
     <x:row r="2" spans="1:4">
       <x:c r="A2" s="0" t="s"/>
     </x:row>
-    <x:row r="3" spans="1:4"/>
-    <x:row r="4" spans="1:4"/>
-    <x:row r="5" spans="1:4"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
@@ -1411,23 +1387,15 @@
     <x:row r="1" spans="1:9">
       <x:c r="A1" s="0" t="s"/>
     </x:row>
-    <x:row r="2" spans="1:9"/>
     <x:row r="3" spans="1:9">
       <x:c r="A3" s="0" t="s"/>
       <x:c r="D3" s="0" t="s"/>
       <x:c r="E3" s="0" t="s"/>
       <x:c r="F3" s="0" t="s"/>
     </x:row>
-    <x:row r="4" spans="1:9"/>
-    <x:row r="5" spans="1:9"/>
-    <x:row r="6" spans="1:9"/>
-    <x:row r="7" spans="1:9"/>
     <x:row r="8" spans="1:9">
       <x:c r="A8" s="0" t="s"/>
     </x:row>
-    <x:row r="9" spans="1:9"/>
-    <x:row r="10" spans="1:9"/>
-    <x:row r="11" spans="1:9"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
@@ -1452,13 +1420,9 @@
     <x:col min="1" max="4" width="9.140625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:4"/>
     <x:row r="2" spans="1:4">
       <x:c r="A2" s="0" t="s"/>
     </x:row>
-    <x:row r="3" spans="1:4"/>
-    <x:row r="4" spans="1:4"/>
-    <x:row r="5" spans="1:4"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
@@ -1483,13 +1447,9 @@
     <x:col min="1" max="4" width="9.140625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:4"/>
     <x:row r="2" spans="1:4">
       <x:c r="A2" s="0" t="s"/>
     </x:row>
-    <x:row r="3" spans="1:4"/>
-    <x:row r="4" spans="1:4"/>
-    <x:row r="5" spans="1:4"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
@@ -1523,9 +1483,6 @@
     <x:row r="3" spans="1:4">
       <x:c r="A3" s="0" t="s"/>
     </x:row>
-    <x:row r="4" spans="1:4"/>
-    <x:row r="5" spans="1:4"/>
-    <x:row r="6" spans="1:4"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
@@ -1553,9 +1510,6 @@
     <x:row r="1" spans="1:4">
       <x:c r="A1" s="0" t="s"/>
     </x:row>
-    <x:row r="2" spans="1:4"/>
-    <x:row r="3" spans="1:4"/>
-    <x:row r="4" spans="1:4"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>

<commit_message>
Update default comment style to be in line with Excel. Change font size to 9pt and disable comment shadow
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Comments/AddingComments.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Comments/AddingComments.xlsx
@@ -35,7 +35,7 @@
         <x:r>
           <x:rPr>
             <x:vertAlign val="baseline"/>
-            <x:sz val="8"/>
+            <x:sz val="9"/>
             <x:color rgb="FF000000"/>
             <x:rFont val="Tahoma"/>
             <x:family val="2"/>
@@ -49,7 +49,7 @@
         <x:r>
           <x:rPr>
             <x:vertAlign val="baseline"/>
-            <x:sz val="8"/>
+            <x:sz val="9"/>
             <x:color rgb="FF000000"/>
             <x:rFont val="Tahoma"/>
             <x:family val="2"/>
@@ -63,7 +63,7 @@
         <x:r>
           <x:rPr>
             <x:vertAlign val="baseline"/>
-            <x:sz val="8"/>
+            <x:sz val="9"/>
             <x:color rgb="FF000000"/>
             <x:rFont val="Tahoma"/>
             <x:family val="2"/>
@@ -77,7 +77,7 @@
         <x:r>
           <x:rPr>
             <x:vertAlign val="baseline"/>
-            <x:sz val="8"/>
+            <x:sz val="9"/>
             <x:color rgb="FF000000"/>
             <x:rFont val="Tahoma"/>
             <x:family val="2"/>
@@ -91,7 +91,7 @@
         <x:r>
           <x:rPr>
             <x:vertAlign val="baseline"/>
-            <x:sz val="8"/>
+            <x:sz val="9"/>
             <x:color rgb="FF000000"/>
             <x:rFont val="Tahoma"/>
             <x:family val="2"/>
@@ -105,7 +105,7 @@
         <x:r>
           <x:rPr>
             <x:vertAlign val="baseline"/>
-            <x:sz val="8"/>
+            <x:sz val="9"/>
             <x:color rgb="FF000000"/>
             <x:rFont val="Tahoma"/>
             <x:family val="2"/>
@@ -120,7 +120,7 @@
           <x:rPr>
             <x:b/>
             <x:vertAlign val="baseline"/>
-            <x:sz val="8"/>
+            <x:sz val="9"/>
             <x:color rgb="FF000000"/>
             <x:rFont val="Tahoma"/>
             <x:family val="2"/>
@@ -130,7 +130,7 @@
         <x:r>
           <x:rPr>
             <x:vertAlign val="baseline"/>
-            <x:sz val="8"/>
+            <x:sz val="9"/>
             <x:color rgb="FF000000"/>
             <x:rFont val="Tahoma"/>
             <x:family val="2"/>
@@ -141,7 +141,7 @@
         <x:r>
           <x:rPr>
             <x:vertAlign val="baseline"/>
-            <x:sz val="8"/>
+            <x:sz val="9"/>
             <x:color rgb="FF000000"/>
             <x:rFont val="Tahoma"/>
             <x:family val="2"/>
@@ -151,7 +151,7 @@
         <x:r>
           <x:rPr>
             <x:vertAlign val="baseline"/>
-            <x:sz val="8"/>
+            <x:sz val="9"/>
             <x:color rgb="FF000000"/>
             <x:rFont val="Tahoma"/>
             <x:family val="2"/>
@@ -162,7 +162,7 @@
         <x:r>
           <x:rPr>
             <x:vertAlign val="baseline"/>
-            <x:sz val="8"/>
+            <x:sz val="9"/>
             <x:color rgb="FF000000"/>
             <x:rFont val="Tahoma"/>
             <x:family val="2"/>
@@ -174,7 +174,7 @@
             <x:b/>
             <x:u val="single"/>
             <x:vertAlign val="baseline"/>
-            <x:sz val="8"/>
+            <x:sz val="9"/>
             <x:color rgb="FFFF355E"/>
             <x:rFont val="Tahoma"/>
             <x:family val="2"/>
@@ -184,7 +184,7 @@
         <x:r>
           <x:rPr>
             <x:vertAlign val="baseline"/>
-            <x:sz val="8"/>
+            <x:sz val="9"/>
             <x:color rgb="FF000000"/>
             <x:rFont val="Tahoma"/>
             <x:family val="2"/>
@@ -198,7 +198,7 @@
         <x:r>
           <x:rPr>
             <x:vertAlign val="baseline"/>
-            <x:sz val="8"/>
+            <x:sz val="9"/>
             <x:color rgb="FF000000"/>
             <x:rFont val="Tahoma"/>
             <x:family val="2"/>
@@ -216,7 +216,7 @@
           <x:rPr>
             <x:b/>
             <x:vertAlign val="baseline"/>
-            <x:sz val="8"/>
+            <x:sz val="9"/>
             <x:color rgb="FF00008B"/>
             <x:rFont val="Tahoma"/>
             <x:family val="2"/>
@@ -227,7 +227,7 @@
           <x:rPr>
             <x:b/>
             <x:vertAlign val="baseline"/>
-            <x:sz val="8"/>
+            <x:sz val="9"/>
             <x:color rgb="FF00008B"/>
             <x:rFont val="Tahoma"/>
             <x:family val="2"/>
@@ -239,7 +239,7 @@
           <x:rPr>
             <x:b/>
             <x:vertAlign val="baseline"/>
-            <x:sz val="8"/>
+            <x:sz val="9"/>
             <x:color rgb="FF00008B"/>
             <x:rFont val="Tahoma"/>
             <x:family val="2"/>
@@ -253,7 +253,7 @@
         <x:r>
           <x:rPr>
             <x:vertAlign val="baseline"/>
-            <x:sz val="8"/>
+            <x:sz val="9"/>
             <x:color rgb="FF000000"/>
             <x:rFont val="Tahoma"/>
             <x:family val="2"/>
@@ -267,7 +267,7 @@
         <x:r>
           <x:rPr>
             <x:vertAlign val="baseline"/>
-            <x:sz val="8"/>
+            <x:sz val="9"/>
             <x:color rgb="FF000000"/>
             <x:rFont val="Tahoma"/>
             <x:family val="2"/>
@@ -281,7 +281,7 @@
         <x:r>
           <x:rPr>
             <x:vertAlign val="baseline"/>
-            <x:sz val="8"/>
+            <x:sz val="9"/>
             <x:color rgb="FF000000"/>
             <x:rFont val="Tahoma"/>
             <x:family val="2"/>
@@ -305,7 +305,7 @@
         <x:r>
           <x:rPr>
             <x:vertAlign val="baseline"/>
-            <x:sz val="8"/>
+            <x:sz val="9"/>
             <x:color rgb="FF000000"/>
             <x:rFont val="Tahoma"/>
             <x:family val="2"/>
@@ -319,7 +319,7 @@
         <x:r>
           <x:rPr>
             <x:vertAlign val="baseline"/>
-            <x:sz val="8"/>
+            <x:sz val="9"/>
             <x:color rgb="FF000000"/>
             <x:rFont val="Tahoma"/>
             <x:family val="2"/>
@@ -333,7 +333,7 @@
         <x:r>
           <x:rPr>
             <x:vertAlign val="baseline"/>
-            <x:sz val="8"/>
+            <x:sz val="9"/>
             <x:color rgb="FF000000"/>
             <x:rFont val="Tahoma"/>
             <x:family val="2"/>
@@ -347,7 +347,7 @@
         <x:r>
           <x:rPr>
             <x:vertAlign val="baseline"/>
-            <x:sz val="8"/>
+            <x:sz val="9"/>
             <x:color rgb="FF000000"/>
             <x:rFont val="Tahoma"/>
             <x:family val="2"/>
@@ -371,7 +371,7 @@
         <x:r>
           <x:rPr>
             <x:vertAlign val="baseline"/>
-            <x:sz val="8"/>
+            <x:sz val="9"/>
             <x:color rgb="FF000000"/>
             <x:rFont val="Tahoma"/>
             <x:family val="2"/>
@@ -396,7 +396,7 @@
           <x:rPr>
             <x:b/>
             <x:vertAlign val="baseline"/>
-            <x:sz val="8"/>
+            <x:sz val="9"/>
             <x:color rgb="FF000000"/>
             <x:rFont val="Tahoma"/>
             <x:family val="2"/>
@@ -406,7 +406,7 @@
         <x:r>
           <x:rPr>
             <x:vertAlign val="baseline"/>
-            <x:sz val="8"/>
+            <x:sz val="9"/>
             <x:color rgb="FF000000"/>
             <x:rFont val="Tahoma"/>
             <x:family val="2"/>
@@ -417,7 +417,7 @@
         <x:r>
           <x:rPr>
             <x:vertAlign val="baseline"/>
-            <x:sz val="8"/>
+            <x:sz val="9"/>
             <x:color rgb="FF000000"/>
             <x:rFont val="Tahoma"/>
             <x:family val="2"/>
@@ -441,7 +441,7 @@
         <x:r>
           <x:rPr>
             <x:vertAlign val="baseline"/>
-            <x:sz val="8"/>
+            <x:sz val="9"/>
             <x:color rgb="FF000000"/>
             <x:rFont val="Tahoma"/>
             <x:family val="2"/>
@@ -455,7 +455,7 @@
         <x:r>
           <x:rPr>
             <x:vertAlign val="baseline"/>
-            <x:sz val="8"/>
+            <x:sz val="9"/>
             <x:color rgb="FF000000"/>
             <x:rFont val="Tahoma"/>
             <x:family val="2"/>
@@ -465,7 +465,7 @@
         <x:r>
           <x:rPr>
             <x:vertAlign val="baseline"/>
-            <x:sz val="8"/>
+            <x:sz val="9"/>
             <x:color rgb="FF000000"/>
             <x:rFont val="Tahoma"/>
             <x:family val="2"/>
@@ -476,7 +476,7 @@
         <x:r>
           <x:rPr>
             <x:vertAlign val="baseline"/>
-            <x:sz val="8"/>
+            <x:sz val="9"/>
             <x:color rgb="FF000000"/>
             <x:rFont val="Tahoma"/>
             <x:family val="2"/>
@@ -486,7 +486,7 @@
         <x:r>
           <x:rPr>
             <x:vertAlign val="baseline"/>
-            <x:sz val="8"/>
+            <x:sz val="9"/>
             <x:color rgb="FF000000"/>
             <x:rFont val="Tahoma"/>
             <x:family val="2"/>
@@ -497,7 +497,7 @@
         <x:r>
           <x:rPr>
             <x:vertAlign val="baseline"/>
-            <x:sz val="8"/>
+            <x:sz val="9"/>
             <x:color rgb="FF000000"/>
             <x:rFont val="Tahoma"/>
             <x:family val="2"/>
@@ -507,7 +507,7 @@
         <x:r>
           <x:rPr>
             <x:vertAlign val="baseline"/>
-            <x:sz val="8"/>
+            <x:sz val="9"/>
             <x:color rgb="FF000000"/>
             <x:rFont val="Tahoma"/>
             <x:family val="2"/>
@@ -518,7 +518,7 @@
         <x:r>
           <x:rPr>
             <x:vertAlign val="baseline"/>
-            <x:sz val="8"/>
+            <x:sz val="9"/>
             <x:color rgb="FF000000"/>
             <x:rFont val="Tahoma"/>
             <x:family val="2"/>
@@ -532,7 +532,7 @@
         <x:r>
           <x:rPr>
             <x:vertAlign val="baseline"/>
-            <x:sz val="8"/>
+            <x:sz val="9"/>
             <x:color rgb="FF000000"/>
             <x:rFont val="Tahoma"/>
             <x:family val="2"/>
@@ -546,7 +546,7 @@
         <x:r>
           <x:rPr>
             <x:vertAlign val="baseline"/>
-            <x:sz val="8"/>
+            <x:sz val="9"/>
             <x:color rgb="FF000000"/>
             <x:rFont val="Tahoma"/>
             <x:family val="2"/>
@@ -560,7 +560,7 @@
         <x:r>
           <x:rPr>
             <x:vertAlign val="baseline"/>
-            <x:sz val="8"/>
+            <x:sz val="9"/>
             <x:color rgb="FF000000"/>
             <x:rFont val="Tahoma"/>
             <x:family val="2"/>
@@ -574,7 +574,7 @@
         <x:r>
           <x:rPr>
             <x:vertAlign val="baseline"/>
-            <x:sz val="8"/>
+            <x:sz val="9"/>
             <x:color rgb="FF000000"/>
             <x:rFont val="Tahoma"/>
             <x:family val="2"/>
@@ -584,7 +584,7 @@
         <x:r>
           <x:rPr>
             <x:vertAlign val="baseline"/>
-            <x:sz val="8"/>
+            <x:sz val="9"/>
             <x:color rgb="FF000000"/>
             <x:rFont val="Tahoma"/>
             <x:family val="2"/>
@@ -595,7 +595,7 @@
         <x:r>
           <x:rPr>
             <x:vertAlign val="baseline"/>
-            <x:sz val="8"/>
+            <x:sz val="9"/>
             <x:color rgb="FF000000"/>
             <x:rFont val="Tahoma"/>
             <x:family val="2"/>
@@ -619,7 +619,7 @@
         <x:r>
           <x:rPr>
             <x:vertAlign val="baseline"/>
-            <x:sz val="8"/>
+            <x:sz val="9"/>
             <x:color rgb="FF000000"/>
             <x:rFont val="Tahoma"/>
             <x:family val="2"/>
@@ -630,7 +630,7 @@
           <x:rPr>
             <x:b/>
             <x:vertAlign val="baseline"/>
-            <x:sz val="8"/>
+            <x:sz val="9"/>
             <x:color rgb="FFFF0000"/>
             <x:rFont val="Tahoma"/>
             <x:family val="2"/>
@@ -640,7 +640,7 @@
         <x:r>
           <x:rPr>
             <x:vertAlign val="baseline"/>
-            <x:sz val="8"/>
+            <x:sz val="9"/>
             <x:color rgb="FF000000"/>
             <x:rFont val="Tahoma"/>
             <x:family val="2"/>
@@ -664,7 +664,7 @@
         <x:r>
           <x:rPr>
             <x:vertAlign val="baseline"/>
-            <x:sz val="8"/>
+            <x:sz val="9"/>
             <x:color rgb="FF000000"/>
             <x:rFont val="Tahoma"/>
             <x:family val="2"/>
@@ -674,7 +674,7 @@
         <x:r>
           <x:rPr>
             <x:vertAlign val="baseline"/>
-            <x:sz val="8"/>
+            <x:sz val="9"/>
             <x:color rgb="FF000000"/>
             <x:rFont val="Tahoma"/>
             <x:family val="2"/>
@@ -685,7 +685,7 @@
         <x:r>
           <x:rPr>
             <x:vertAlign val="baseline"/>
-            <x:sz val="8"/>
+            <x:sz val="9"/>
             <x:color rgb="FF000000"/>
             <x:rFont val="Tahoma"/>
             <x:family val="2"/>
@@ -695,7 +695,7 @@
         <x:r>
           <x:rPr>
             <x:vertAlign val="baseline"/>
-            <x:sz val="8"/>
+            <x:sz val="9"/>
             <x:color rgb="FF000000"/>
             <x:rFont val="Tahoma"/>
             <x:family val="2"/>
@@ -706,7 +706,7 @@
         <x:r>
           <x:rPr>
             <x:vertAlign val="baseline"/>
-            <x:sz val="8"/>
+            <x:sz val="9"/>
             <x:color rgb="FF000000"/>
             <x:rFont val="Tahoma"/>
             <x:family val="2"/>
@@ -762,7 +762,7 @@
         <x:r>
           <x:rPr>
             <x:vertAlign val="baseline"/>
-            <x:sz val="8"/>
+            <x:sz val="9"/>
             <x:color rgb="FF000000"/>
             <x:rFont val="Tahoma"/>
             <x:family val="2"/>
@@ -776,7 +776,7 @@
         <x:r>
           <x:rPr>
             <x:vertAlign val="baseline"/>
-            <x:sz val="8"/>
+            <x:sz val="9"/>
             <x:color rgb="FF000000"/>
             <x:rFont val="Tahoma"/>
             <x:family val="2"/>

</xml_diff>

<commit_message>
Refactor reading and writing of Comments Ensure comment shapeID remains consistent across saves
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Comments/AddingComments.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Comments/AddingComments.xlsx
@@ -23,7 +23,7 @@
 </x:workbook>
 </file>
 
-<file path=xl/comments12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:comments xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:authors>
     <x:author>Manuel</x:author>
@@ -294,321 +294,7 @@
 </x:comments>
 </file>
 
-<file path=xl/comments13.xml><?xml version="1.0" encoding="utf-8"?>
-<x:comments xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:authors>
-    <x:author>Manuel</x:author>
-  </x:authors>
-  <x:commentList>
-    <x:comment ref="A1" authorId="0">
-      <x:text>
-        <x:r>
-          <x:rPr>
-            <x:vertAlign val="baseline"/>
-            <x:sz val="9"/>
-            <x:color rgb="FF000000"/>
-            <x:rFont val="Tahoma"/>
-            <x:family val="2"/>
-          </x:rPr>
-          <x:t>Hidden</x:t>
-        </x:r>
-      </x:text>
-    </x:comment>
-    <x:comment ref="A2" authorId="0">
-      <x:text>
-        <x:r>
-          <x:rPr>
-            <x:vertAlign val="baseline"/>
-            <x:sz val="9"/>
-            <x:color rgb="FF000000"/>
-            <x:rFont val="Tahoma"/>
-            <x:family val="2"/>
-          </x:rPr>
-          <x:t>Visible</x:t>
-        </x:r>
-      </x:text>
-    </x:comment>
-    <x:comment ref="A3" authorId="0">
-      <x:text>
-        <x:r>
-          <x:rPr>
-            <x:vertAlign val="baseline"/>
-            <x:sz val="9"/>
-            <x:color rgb="FF000000"/>
-            <x:rFont val="Tahoma"/>
-            <x:family val="2"/>
-          </x:rPr>
-          <x:t>On Top</x:t>
-        </x:r>
-      </x:text>
-    </x:comment>
-    <x:comment ref="A4" authorId="0">
-      <x:text>
-        <x:r>
-          <x:rPr>
-            <x:vertAlign val="baseline"/>
-            <x:sz val="9"/>
-            <x:color rgb="FF000000"/>
-            <x:rFont val="Tahoma"/>
-            <x:family val="2"/>
-          </x:rPr>
-          <x:t>Underneath</x:t>
-        </x:r>
-      </x:text>
-    </x:comment>
-  </x:commentList>
-</x:comments>
-</file>
-
-<file path=xl/comments14.xml><?xml version="1.0" encoding="utf-8"?>
-<x:comments xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:authors>
-    <x:author>Manuel</x:author>
-  </x:authors>
-  <x:commentList>
-    <x:comment ref="A1" authorId="0">
-      <x:text>
-        <x:r>
-          <x:rPr>
-            <x:vertAlign val="baseline"/>
-            <x:sz val="9"/>
-            <x:color rgb="FF000000"/>
-            <x:rFont val="Tahoma"/>
-            <x:family val="2"/>
-          </x:rPr>
-          <x:t>This is an unusual place for a comment...</x:t>
-        </x:r>
-      </x:text>
-    </x:comment>
-  </x:commentList>
-</x:comments>
-</file>
-
-<file path=xl/comments15.xml><?xml version="1.0" encoding="utf-8"?>
-<x:comments xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:authors>
-    <x:author>MDeLeon</x:author>
-  </x:authors>
-  <x:commentList>
-    <x:comment ref="A2" authorId="0">
-      <x:text>
-        <x:r>
-          <x:rPr>
-            <x:b/>
-            <x:vertAlign val="baseline"/>
-            <x:sz val="9"/>
-            <x:color rgb="FF000000"/>
-            <x:rFont val="Tahoma"/>
-            <x:family val="2"/>
-          </x:rPr>
-          <x:t>MDeLeon:</x:t>
-        </x:r>
-        <x:r>
-          <x:rPr>
-            <x:vertAlign val="baseline"/>
-            <x:sz val="9"/>
-            <x:color rgb="FF000000"/>
-            <x:rFont val="Tahoma"/>
-            <x:family val="2"/>
-          </x:rPr>
-          <x:t xml:space="preserve">
-</x:t>
-        </x:r>
-        <x:r>
-          <x:rPr>
-            <x:vertAlign val="baseline"/>
-            <x:sz val="9"/>
-            <x:color rgb="FF000000"/>
-            <x:rFont val="Tahoma"/>
-            <x:family val="2"/>
-          </x:rPr>
-          <x:t>Hello World!</x:t>
-        </x:r>
-      </x:text>
-    </x:comment>
-  </x:commentList>
-</x:comments>
-</file>
-
-<file path=xl/comments16.xml><?xml version="1.0" encoding="utf-8"?>
-<x:comments xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:authors>
-    <x:author>Manuel</x:author>
-  </x:authors>
-  <x:commentList>
-    <x:comment ref="A1" authorId="0">
-      <x:text>
-        <x:r>
-          <x:rPr>
-            <x:vertAlign val="baseline"/>
-            <x:sz val="9"/>
-            <x:color rgb="FF000000"/>
-            <x:rFont val="Tahoma"/>
-            <x:family val="2"/>
-          </x:rPr>
-          <x:t>Things are pretty tight around here</x:t>
-        </x:r>
-      </x:text>
-    </x:comment>
-    <x:comment ref="A3" authorId="0">
-      <x:text>
-        <x:r>
-          <x:rPr>
-            <x:vertAlign val="baseline"/>
-            <x:sz val="9"/>
-            <x:color rgb="FF000000"/>
-            <x:rFont val="Tahoma"/>
-            <x:family val="2"/>
-          </x:rPr>
-          <x:t>Default Alignments:</x:t>
-        </x:r>
-        <x:r>
-          <x:rPr>
-            <x:vertAlign val="baseline"/>
-            <x:sz val="9"/>
-            <x:color rgb="FF000000"/>
-            <x:rFont val="Tahoma"/>
-            <x:family val="2"/>
-          </x:rPr>
-          <x:t xml:space="preserve">
-</x:t>
-        </x:r>
-        <x:r>
-          <x:rPr>
-            <x:vertAlign val="baseline"/>
-            <x:sz val="9"/>
-            <x:color rgb="FF000000"/>
-            <x:rFont val="Tahoma"/>
-            <x:family val="2"/>
-          </x:rPr>
-          <x:t>Vertical = Top</x:t>
-        </x:r>
-        <x:r>
-          <x:rPr>
-            <x:vertAlign val="baseline"/>
-            <x:sz val="9"/>
-            <x:color rgb="FF000000"/>
-            <x:rFont val="Tahoma"/>
-            <x:family val="2"/>
-          </x:rPr>
-          <x:t xml:space="preserve">
-</x:t>
-        </x:r>
-        <x:r>
-          <x:rPr>
-            <x:vertAlign val="baseline"/>
-            <x:sz val="9"/>
-            <x:color rgb="FF000000"/>
-            <x:rFont val="Tahoma"/>
-            <x:family val="2"/>
-          </x:rPr>
-          <x:t>Horizontal = Left</x:t>
-        </x:r>
-        <x:r>
-          <x:rPr>
-            <x:vertAlign val="baseline"/>
-            <x:sz val="9"/>
-            <x:color rgb="FF000000"/>
-            <x:rFont val="Tahoma"/>
-            <x:family val="2"/>
-          </x:rPr>
-          <x:t xml:space="preserve">
-</x:t>
-        </x:r>
-        <x:r>
-          <x:rPr>
-            <x:vertAlign val="baseline"/>
-            <x:sz val="9"/>
-            <x:color rgb="FF000000"/>
-            <x:rFont val="Tahoma"/>
-            <x:family val="2"/>
-          </x:rPr>
-          <x:t>Orientation = Left to Right</x:t>
-        </x:r>
-      </x:text>
-    </x:comment>
-    <x:comment ref="D3" authorId="0">
-      <x:text>
-        <x:r>
-          <x:rPr>
-            <x:vertAlign val="baseline"/>
-            <x:sz val="9"/>
-            <x:color rgb="FF000000"/>
-            <x:rFont val="Tahoma"/>
-            <x:family val="2"/>
-          </x:rPr>
-          <x:t>Orientation = Bottom to Top</x:t>
-        </x:r>
-      </x:text>
-    </x:comment>
-    <x:comment ref="E3" authorId="0">
-      <x:text>
-        <x:r>
-          <x:rPr>
-            <x:vertAlign val="baseline"/>
-            <x:sz val="9"/>
-            <x:color rgb="FF000000"/>
-            <x:rFont val="Tahoma"/>
-            <x:family val="2"/>
-          </x:rPr>
-          <x:t>Orientation = Top to Bottom</x:t>
-        </x:r>
-      </x:text>
-    </x:comment>
-    <x:comment ref="F3" authorId="0">
-      <x:text>
-        <x:r>
-          <x:rPr>
-            <x:vertAlign val="baseline"/>
-            <x:sz val="9"/>
-            <x:color rgb="FF000000"/>
-            <x:rFont val="Tahoma"/>
-            <x:family val="2"/>
-          </x:rPr>
-          <x:t>Orientation = Vertical</x:t>
-        </x:r>
-      </x:text>
-    </x:comment>
-    <x:comment ref="A8" authorId="0">
-      <x:text>
-        <x:r>
-          <x:rPr>
-            <x:vertAlign val="baseline"/>
-            <x:sz val="9"/>
-            <x:color rgb="FF000000"/>
-            <x:rFont val="Tahoma"/>
-            <x:family val="2"/>
-          </x:rPr>
-          <x:t>Vertical = Bottom</x:t>
-        </x:r>
-        <x:r>
-          <x:rPr>
-            <x:vertAlign val="baseline"/>
-            <x:sz val="9"/>
-            <x:color rgb="FF000000"/>
-            <x:rFont val="Tahoma"/>
-            <x:family val="2"/>
-          </x:rPr>
-          <x:t xml:space="preserve">
-</x:t>
-        </x:r>
-        <x:r>
-          <x:rPr>
-            <x:vertAlign val="baseline"/>
-            <x:sz val="9"/>
-            <x:color rgb="FF000000"/>
-            <x:rFont val="Tahoma"/>
-            <x:family val="2"/>
-          </x:rPr>
-          <x:t>Horizontal = Right</x:t>
-        </x:r>
-      </x:text>
-    </x:comment>
-  </x:commentList>
-</x:comments>
-</file>
-
-<file path=xl/comments17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments10.xml><?xml version="1.0" encoding="utf-8"?>
 <x:comments xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:authors>
     <x:author>Manuel</x:author>
@@ -624,28 +310,21 @@
             <x:rFont val="Tahoma"/>
             <x:family val="2"/>
           </x:rPr>
-          <x:t xml:space="preserve">Now </x:t>
-        </x:r>
-        <x:r>
-          <x:rPr>
-            <x:b/>
-            <x:vertAlign val="baseline"/>
-            <x:sz val="9"/>
-            <x:color rgb="FFFF0000"/>
-            <x:rFont val="Tahoma"/>
-            <x:family val="2"/>
-          </x:rPr>
-          <x:t>THIS</x:t>
-        </x:r>
-        <x:r>
-          <x:rPr>
-            <x:vertAlign val="baseline"/>
-            <x:sz val="9"/>
-            <x:color rgb="FF000000"/>
-            <x:rFont val="Tahoma"/>
-            <x:family val="2"/>
-          </x:rPr>
-          <x:t xml:space="preserve"> is colorful!</x:t>
+          <x:t>Things are very tight around here.</x:t>
+        </x:r>
+      </x:text>
+    </x:comment>
+    <x:comment ref="A4" authorId="0">
+      <x:text>
+        <x:r>
+          <x:rPr>
+            <x:vertAlign val="baseline"/>
+            <x:sz val="9"/>
+            <x:color rgb="FF000000"/>
+            <x:rFont val="Tahoma"/>
+            <x:family val="2"/>
+          </x:rPr>
+          <x:t>Different size</x:t>
         </x:r>
       </x:text>
     </x:comment>
@@ -653,73 +332,7 @@
 </x:comments>
 </file>
 
-<file path=xl/comments18.xml><?xml version="1.0" encoding="utf-8"?>
-<x:comments xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:authors>
-    <x:author>Manuel</x:author>
-  </x:authors>
-  <x:commentList>
-    <x:comment ref="A2" authorId="0">
-      <x:text>
-        <x:r>
-          <x:rPr>
-            <x:vertAlign val="baseline"/>
-            <x:sz val="9"/>
-            <x:color rgb="FF000000"/>
-            <x:rFont val="Tahoma"/>
-            <x:family val="2"/>
-          </x:rPr>
-          <x:t xml:space="preserve">Lorem ipsum dolor sit amet, adipiscing elit. </x:t>
-        </x:r>
-        <x:r>
-          <x:rPr>
-            <x:vertAlign val="baseline"/>
-            <x:sz val="9"/>
-            <x:color rgb="FF000000"/>
-            <x:rFont val="Tahoma"/>
-            <x:family val="2"/>
-          </x:rPr>
-          <x:t xml:space="preserve">
-</x:t>
-        </x:r>
-        <x:r>
-          <x:rPr>
-            <x:vertAlign val="baseline"/>
-            <x:sz val="9"/>
-            <x:color rgb="FF000000"/>
-            <x:rFont val="Tahoma"/>
-            <x:family val="2"/>
-          </x:rPr>
-          <x:t xml:space="preserve">Nunc elementum, sapien a ultrices, commodo nisl. </x:t>
-        </x:r>
-        <x:r>
-          <x:rPr>
-            <x:vertAlign val="baseline"/>
-            <x:sz val="9"/>
-            <x:color rgb="FF000000"/>
-            <x:rFont val="Tahoma"/>
-            <x:family val="2"/>
-          </x:rPr>
-          <x:t xml:space="preserve">
-</x:t>
-        </x:r>
-        <x:r>
-          <x:rPr>
-            <x:vertAlign val="baseline"/>
-            <x:sz val="9"/>
-            <x:color rgb="FF000000"/>
-            <x:rFont val="Tahoma"/>
-            <x:family val="2"/>
-          </x:rPr>
-          <x:t>Consequat erat lectus a nisi. Aliquam facilisis.</x:t>
-        </x:r>
-      </x:text>
-    </x:comment>
-  </x:commentList>
-</x:comments>
-</file>
-
-<file path=xl/comments19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments11.xml><?xml version="1.0" encoding="utf-8"?>
 <x:comments xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:authors>
     <x:author>Manuel</x:author>
@@ -728,17 +341,436 @@
     <x:comment ref="A1" authorId="0">
       <x:text/>
     </x:comment>
-    <x:comment ref="A2" authorId="0">
-      <x:text/>
-    </x:comment>
-    <x:comment ref="A3" authorId="0">
-      <x:text/>
-    </x:comment>
   </x:commentList>
 </x:comments>
 </file>
 
-<file path=xl/comments20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<x:comments xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:authors>
+    <x:author>Manuel</x:author>
+  </x:authors>
+  <x:commentList>
+    <x:comment ref="A1" authorId="0">
+      <x:text>
+        <x:r>
+          <x:rPr>
+            <x:vertAlign val="baseline"/>
+            <x:sz val="9"/>
+            <x:color rgb="FF000000"/>
+            <x:rFont val="Tahoma"/>
+            <x:family val="2"/>
+          </x:rPr>
+          <x:t>Hidden</x:t>
+        </x:r>
+      </x:text>
+    </x:comment>
+    <x:comment ref="A2" authorId="0">
+      <x:text>
+        <x:r>
+          <x:rPr>
+            <x:vertAlign val="baseline"/>
+            <x:sz val="9"/>
+            <x:color rgb="FF000000"/>
+            <x:rFont val="Tahoma"/>
+            <x:family val="2"/>
+          </x:rPr>
+          <x:t>Visible</x:t>
+        </x:r>
+      </x:text>
+    </x:comment>
+    <x:comment ref="A3" authorId="0">
+      <x:text>
+        <x:r>
+          <x:rPr>
+            <x:vertAlign val="baseline"/>
+            <x:sz val="9"/>
+            <x:color rgb="FF000000"/>
+            <x:rFont val="Tahoma"/>
+            <x:family val="2"/>
+          </x:rPr>
+          <x:t>On Top</x:t>
+        </x:r>
+      </x:text>
+    </x:comment>
+    <x:comment ref="A4" authorId="0">
+      <x:text>
+        <x:r>
+          <x:rPr>
+            <x:vertAlign val="baseline"/>
+            <x:sz val="9"/>
+            <x:color rgb="FF000000"/>
+            <x:rFont val="Tahoma"/>
+            <x:family val="2"/>
+          </x:rPr>
+          <x:t>Underneath</x:t>
+        </x:r>
+      </x:text>
+    </x:comment>
+  </x:commentList>
+</x:comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<x:comments xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:authors>
+    <x:author>Manuel</x:author>
+  </x:authors>
+  <x:commentList>
+    <x:comment ref="A1" authorId="0">
+      <x:text>
+        <x:r>
+          <x:rPr>
+            <x:vertAlign val="baseline"/>
+            <x:sz val="9"/>
+            <x:color rgb="FF000000"/>
+            <x:rFont val="Tahoma"/>
+            <x:family val="2"/>
+          </x:rPr>
+          <x:t>This is an unusual place for a comment...</x:t>
+        </x:r>
+      </x:text>
+    </x:comment>
+  </x:commentList>
+</x:comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<x:comments xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:authors>
+    <x:author>MDeLeon</x:author>
+  </x:authors>
+  <x:commentList>
+    <x:comment ref="A2" authorId="0">
+      <x:text>
+        <x:r>
+          <x:rPr>
+            <x:b/>
+            <x:vertAlign val="baseline"/>
+            <x:sz val="9"/>
+            <x:color rgb="FF000000"/>
+            <x:rFont val="Tahoma"/>
+            <x:family val="2"/>
+          </x:rPr>
+          <x:t>MDeLeon:</x:t>
+        </x:r>
+        <x:r>
+          <x:rPr>
+            <x:vertAlign val="baseline"/>
+            <x:sz val="9"/>
+            <x:color rgb="FF000000"/>
+            <x:rFont val="Tahoma"/>
+            <x:family val="2"/>
+          </x:rPr>
+          <x:t xml:space="preserve">
+</x:t>
+        </x:r>
+        <x:r>
+          <x:rPr>
+            <x:vertAlign val="baseline"/>
+            <x:sz val="9"/>
+            <x:color rgb="FF000000"/>
+            <x:rFont val="Tahoma"/>
+            <x:family val="2"/>
+          </x:rPr>
+          <x:t>Hello World!</x:t>
+        </x:r>
+      </x:text>
+    </x:comment>
+  </x:commentList>
+</x:comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<x:comments xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:authors>
+    <x:author>Manuel</x:author>
+  </x:authors>
+  <x:commentList>
+    <x:comment ref="A1" authorId="0">
+      <x:text>
+        <x:r>
+          <x:rPr>
+            <x:vertAlign val="baseline"/>
+            <x:sz val="9"/>
+            <x:color rgb="FF000000"/>
+            <x:rFont val="Tahoma"/>
+            <x:family val="2"/>
+          </x:rPr>
+          <x:t>Things are pretty tight around here</x:t>
+        </x:r>
+      </x:text>
+    </x:comment>
+    <x:comment ref="A3" authorId="0">
+      <x:text>
+        <x:r>
+          <x:rPr>
+            <x:vertAlign val="baseline"/>
+            <x:sz val="9"/>
+            <x:color rgb="FF000000"/>
+            <x:rFont val="Tahoma"/>
+            <x:family val="2"/>
+          </x:rPr>
+          <x:t>Default Alignments:</x:t>
+        </x:r>
+        <x:r>
+          <x:rPr>
+            <x:vertAlign val="baseline"/>
+            <x:sz val="9"/>
+            <x:color rgb="FF000000"/>
+            <x:rFont val="Tahoma"/>
+            <x:family val="2"/>
+          </x:rPr>
+          <x:t xml:space="preserve">
+</x:t>
+        </x:r>
+        <x:r>
+          <x:rPr>
+            <x:vertAlign val="baseline"/>
+            <x:sz val="9"/>
+            <x:color rgb="FF000000"/>
+            <x:rFont val="Tahoma"/>
+            <x:family val="2"/>
+          </x:rPr>
+          <x:t>Vertical = Top</x:t>
+        </x:r>
+        <x:r>
+          <x:rPr>
+            <x:vertAlign val="baseline"/>
+            <x:sz val="9"/>
+            <x:color rgb="FF000000"/>
+            <x:rFont val="Tahoma"/>
+            <x:family val="2"/>
+          </x:rPr>
+          <x:t xml:space="preserve">
+</x:t>
+        </x:r>
+        <x:r>
+          <x:rPr>
+            <x:vertAlign val="baseline"/>
+            <x:sz val="9"/>
+            <x:color rgb="FF000000"/>
+            <x:rFont val="Tahoma"/>
+            <x:family val="2"/>
+          </x:rPr>
+          <x:t>Horizontal = Left</x:t>
+        </x:r>
+        <x:r>
+          <x:rPr>
+            <x:vertAlign val="baseline"/>
+            <x:sz val="9"/>
+            <x:color rgb="FF000000"/>
+            <x:rFont val="Tahoma"/>
+            <x:family val="2"/>
+          </x:rPr>
+          <x:t xml:space="preserve">
+</x:t>
+        </x:r>
+        <x:r>
+          <x:rPr>
+            <x:vertAlign val="baseline"/>
+            <x:sz val="9"/>
+            <x:color rgb="FF000000"/>
+            <x:rFont val="Tahoma"/>
+            <x:family val="2"/>
+          </x:rPr>
+          <x:t>Orientation = Left to Right</x:t>
+        </x:r>
+      </x:text>
+    </x:comment>
+    <x:comment ref="D3" authorId="0">
+      <x:text>
+        <x:r>
+          <x:rPr>
+            <x:vertAlign val="baseline"/>
+            <x:sz val="9"/>
+            <x:color rgb="FF000000"/>
+            <x:rFont val="Tahoma"/>
+            <x:family val="2"/>
+          </x:rPr>
+          <x:t>Orientation = Bottom to Top</x:t>
+        </x:r>
+      </x:text>
+    </x:comment>
+    <x:comment ref="E3" authorId="0">
+      <x:text>
+        <x:r>
+          <x:rPr>
+            <x:vertAlign val="baseline"/>
+            <x:sz val="9"/>
+            <x:color rgb="FF000000"/>
+            <x:rFont val="Tahoma"/>
+            <x:family val="2"/>
+          </x:rPr>
+          <x:t>Orientation = Top to Bottom</x:t>
+        </x:r>
+      </x:text>
+    </x:comment>
+    <x:comment ref="F3" authorId="0">
+      <x:text>
+        <x:r>
+          <x:rPr>
+            <x:vertAlign val="baseline"/>
+            <x:sz val="9"/>
+            <x:color rgb="FF000000"/>
+            <x:rFont val="Tahoma"/>
+            <x:family val="2"/>
+          </x:rPr>
+          <x:t>Orientation = Vertical</x:t>
+        </x:r>
+      </x:text>
+    </x:comment>
+    <x:comment ref="A8" authorId="0">
+      <x:text>
+        <x:r>
+          <x:rPr>
+            <x:vertAlign val="baseline"/>
+            <x:sz val="9"/>
+            <x:color rgb="FF000000"/>
+            <x:rFont val="Tahoma"/>
+            <x:family val="2"/>
+          </x:rPr>
+          <x:t>Vertical = Bottom</x:t>
+        </x:r>
+        <x:r>
+          <x:rPr>
+            <x:vertAlign val="baseline"/>
+            <x:sz val="9"/>
+            <x:color rgb="FF000000"/>
+            <x:rFont val="Tahoma"/>
+            <x:family val="2"/>
+          </x:rPr>
+          <x:t xml:space="preserve">
+</x:t>
+        </x:r>
+        <x:r>
+          <x:rPr>
+            <x:vertAlign val="baseline"/>
+            <x:sz val="9"/>
+            <x:color rgb="FF000000"/>
+            <x:rFont val="Tahoma"/>
+            <x:family val="2"/>
+          </x:rPr>
+          <x:t>Horizontal = Right</x:t>
+        </x:r>
+      </x:text>
+    </x:comment>
+  </x:commentList>
+</x:comments>
+</file>
+
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<x:comments xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:authors>
+    <x:author>Manuel</x:author>
+  </x:authors>
+  <x:commentList>
+    <x:comment ref="A2" authorId="0">
+      <x:text>
+        <x:r>
+          <x:rPr>
+            <x:vertAlign val="baseline"/>
+            <x:sz val="9"/>
+            <x:color rgb="FF000000"/>
+            <x:rFont val="Tahoma"/>
+            <x:family val="2"/>
+          </x:rPr>
+          <x:t xml:space="preserve">Now </x:t>
+        </x:r>
+        <x:r>
+          <x:rPr>
+            <x:b/>
+            <x:vertAlign val="baseline"/>
+            <x:sz val="9"/>
+            <x:color rgb="FFFF0000"/>
+            <x:rFont val="Tahoma"/>
+            <x:family val="2"/>
+          </x:rPr>
+          <x:t>THIS</x:t>
+        </x:r>
+        <x:r>
+          <x:rPr>
+            <x:vertAlign val="baseline"/>
+            <x:sz val="9"/>
+            <x:color rgb="FF000000"/>
+            <x:rFont val="Tahoma"/>
+            <x:family val="2"/>
+          </x:rPr>
+          <x:t xml:space="preserve"> is colorful!</x:t>
+        </x:r>
+      </x:text>
+    </x:comment>
+  </x:commentList>
+</x:comments>
+</file>
+
+<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
+<x:comments xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:authors>
+    <x:author>Manuel</x:author>
+  </x:authors>
+  <x:commentList>
+    <x:comment ref="A2" authorId="0">
+      <x:text>
+        <x:r>
+          <x:rPr>
+            <x:vertAlign val="baseline"/>
+            <x:sz val="9"/>
+            <x:color rgb="FF000000"/>
+            <x:rFont val="Tahoma"/>
+            <x:family val="2"/>
+          </x:rPr>
+          <x:t xml:space="preserve">Lorem ipsum dolor sit amet, adipiscing elit. </x:t>
+        </x:r>
+        <x:r>
+          <x:rPr>
+            <x:vertAlign val="baseline"/>
+            <x:sz val="9"/>
+            <x:color rgb="FF000000"/>
+            <x:rFont val="Tahoma"/>
+            <x:family val="2"/>
+          </x:rPr>
+          <x:t xml:space="preserve">
+</x:t>
+        </x:r>
+        <x:r>
+          <x:rPr>
+            <x:vertAlign val="baseline"/>
+            <x:sz val="9"/>
+            <x:color rgb="FF000000"/>
+            <x:rFont val="Tahoma"/>
+            <x:family val="2"/>
+          </x:rPr>
+          <x:t xml:space="preserve">Nunc elementum, sapien a ultrices, commodo nisl. </x:t>
+        </x:r>
+        <x:r>
+          <x:rPr>
+            <x:vertAlign val="baseline"/>
+            <x:sz val="9"/>
+            <x:color rgb="FF000000"/>
+            <x:rFont val="Tahoma"/>
+            <x:family val="2"/>
+          </x:rPr>
+          <x:t xml:space="preserve">
+</x:t>
+        </x:r>
+        <x:r>
+          <x:rPr>
+            <x:vertAlign val="baseline"/>
+            <x:sz val="9"/>
+            <x:color rgb="FF000000"/>
+            <x:rFont val="Tahoma"/>
+            <x:family val="2"/>
+          </x:rPr>
+          <x:t>Consequat erat lectus a nisi. Aliquam facilisis.</x:t>
+        </x:r>
+      </x:text>
+    </x:comment>
+  </x:commentList>
+</x:comments>
+</file>
+
+<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
 <x:comments xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:authors>
     <x:author>Manuel</x:author>
@@ -747,49 +779,17 @@
     <x:comment ref="A1" authorId="0">
       <x:text/>
     </x:comment>
+    <x:comment ref="A2" authorId="0">
+      <x:text/>
+    </x:comment>
+    <x:comment ref="A3" authorId="0">
+      <x:text/>
+    </x:comment>
   </x:commentList>
 </x:comments>
 </file>
 
-<file path=xl/comments21.xml><?xml version="1.0" encoding="utf-8"?>
-<x:comments xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:authors>
-    <x:author>Manuel</x:author>
-  </x:authors>
-  <x:commentList>
-    <x:comment ref="A2" authorId="0">
-      <x:text>
-        <x:r>
-          <x:rPr>
-            <x:vertAlign val="baseline"/>
-            <x:sz val="9"/>
-            <x:color rgb="FF000000"/>
-            <x:rFont val="Tahoma"/>
-            <x:family val="2"/>
-          </x:rPr>
-          <x:t>Things are very tight around here.</x:t>
-        </x:r>
-      </x:text>
-    </x:comment>
-    <x:comment ref="A4" authorId="0">
-      <x:text>
-        <x:r>
-          <x:rPr>
-            <x:vertAlign val="baseline"/>
-            <x:sz val="9"/>
-            <x:color rgb="FF000000"/>
-            <x:rFont val="Tahoma"/>
-            <x:family val="2"/>
-          </x:rPr>
-          <x:t>Different size</x:t>
-        </x:r>
-      </x:text>
-    </x:comment>
-  </x:commentList>
-</x:comments>
-</file>
-
-<file path=xl/comments22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
 <x:comments xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:authors>
     <x:author>Manuel</x:author>

</xml_diff>